<commit_message>
veel code toegevoegd aangezien ik vergeten was
</commit_message>
<xml_diff>
--- a/algemeen/logboek.xlsx
+++ b/algemeen/logboek.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thijn\Documents\school\_MA\Bewijzenmap\Leerjaar-02\Periode02\BO\algemeen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F06A49BD-8041-481D-9902-DCF8073D0720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE4A7B8-BB70-4B8D-B680-AACFCB1676E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F82D63F8-D999-417B-9A2E-4237B9912B6E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>vandaag heb ik het idee bedacht voor wat we wouden doen. Ik heb de github en de trello opgezet. Daarnaast heb ik de excel voor het logboek aangemaakt.</t>
   </si>
@@ -58,6 +58,33 @@
   </si>
   <si>
     <t>vandaag ben ik bezig geweest met de materiaal lijst maken en kijken of we het redden met de kosten.</t>
+  </si>
+  <si>
+    <t>vandaag ben ik de lessen gevolgd en nog wat onderzoek gedaan</t>
+  </si>
+  <si>
+    <t>vandaag heb ik de lessen gevolgd van ed en ben verder gegaan met onderzoek naar het project</t>
+  </si>
+  <si>
+    <t>vandaag heb ik de informatie pagina van  onze kunstenaar gemaakt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vandaag heb ik een begin gemaakt aan de form pagina </t>
+  </si>
+  <si>
+    <t>studiedag</t>
+  </si>
+  <si>
+    <t>vrij</t>
+  </si>
+  <si>
+    <t>vandaag heb ik met mijn team bedacht wat we nog meer nodig hadden qua spullen</t>
+  </si>
+  <si>
+    <t>vandaag heb ik de spullen gehaald met elisa gehaald zoals hout en kippengaas enzo</t>
+  </si>
+  <si>
+    <t>vandaag heb ik onderzoek gedaan naar database en form</t>
   </si>
 </sst>
 </file>
@@ -410,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9C3EC51-DD40-4511-9E0A-AA63B85F0A1E}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,6 +502,110 @@
       </c>
       <c r="B8" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>44898</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>44901</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>44902</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>44903</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>44904</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>44905</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>44908</v>
+      </c>
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>44909</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>44910</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>44911</v>
+      </c>
+      <c r="B21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>44912</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>44906</v>
+      </c>
+      <c r="B24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>44907</v>
       </c>
     </row>
   </sheetData>

</xml_diff>